<commit_message>
changed oneway weekend surcharge calculation
</commit_message>
<xml_diff>
--- a/python/FareFiling/fare_input_backup.xlsx
+++ b/python/FareFiling/fare_input_backup.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="L" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="K1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="K2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="H1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="H2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="P" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="L" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="K1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="K2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="H1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="H2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="P" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
added season mapping O for one season
</commit_message>
<xml_diff>
--- a/python/FareFiling/fare_input_backup.xlsx
+++ b/python/FareFiling/fare_input_backup.xlsx
@@ -12,6 +12,7 @@
     <sheet name="H1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="H2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="P" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="O" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -518,7 +519,6 @@
       <c r="D2" t="n">
         <v>2300</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -539,7 +539,6 @@
       <c r="D3" t="n">
         <v>2400</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,7 +559,6 @@
       <c r="D4" t="n">
         <v>3100</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -581,7 +579,6 @@
       <c r="D5" t="n">
         <v>3200</v>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -602,7 +599,6 @@
       <c r="D6" t="n">
         <v>3900</v>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -623,7 +619,6 @@
       <c r="D7" t="n">
         <v>4000</v>
       </c>
-      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -690,7 +685,6 @@
       <c r="D2" t="n">
         <v>2500</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -711,7 +705,6 @@
       <c r="D3" t="n">
         <v>2600</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -732,7 +725,6 @@
       <c r="D4" t="n">
         <v>3300</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -799,7 +791,6 @@
       <c r="D2" t="n">
         <v>3400</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -820,7 +811,6 @@
       <c r="D3" t="n">
         <v>4100</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -841,7 +831,6 @@
       <c r="D4" t="n">
         <v>4200</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -908,7 +897,6 @@
       <c r="D2" t="n">
         <v>2700</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -929,7 +917,6 @@
       <c r="D3" t="n">
         <v>2800</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -950,7 +937,6 @@
       <c r="D4" t="n">
         <v>3500</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1017,7 +1003,6 @@
       <c r="D2" t="n">
         <v>3600</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1038,7 +1023,6 @@
       <c r="D3" t="n">
         <v>4300</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1059,7 +1043,6 @@
       <c r="D4" t="n">
         <v>4400</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1126,7 +1109,6 @@
       <c r="D2" t="n">
         <v>2900</v>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1147,7 +1129,6 @@
       <c r="D3" t="n">
         <v>3000</v>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1168,7 +1149,6 @@
       <c r="D4" t="n">
         <v>3700</v>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1189,7 +1169,6 @@
       <c r="D5" t="n">
         <v>3800</v>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1210,7 +1189,680 @@
       <c r="D6" t="n">
         <v>4500</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>dest</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>booking_class</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>season</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>base_fare</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Unnamed: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Remarks:
+'O' for One Season</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2400</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2600</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>U</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2700</v>
+      </c>
       <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2800</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2900</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TPE</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3100</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3200</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3400</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3500</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>U</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3600</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>3700</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SGN</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>3800</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3900</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4100</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4200</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>U</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4300</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4400</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BKK</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4500</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>